<commit_message>
corrected buttons, new relocation
</commit_message>
<xml_diff>
--- a/Zayavki.xlsx
+++ b/Zayavki.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,37 +436,17 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>ФИО</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Адрес</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
           <t>Телефон</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1899059721</v>
+        <v>1149518006</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Абв Где Жзи</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Улица бабайка,дом 13, КВ 6</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>+7900000000</t>
+          <t>+73452598001</t>
         </is>
       </c>
     </row>

</xml_diff>